<commit_message>
4/24 - complete run
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ScrappedRecipes.xlsx
+++ b/src/test/resources/TestData/ScrappedRecipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2146cd726dde662f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D906ED84-7061-4FDC-94CB-6DCD48924DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{D906ED84-7061-4FDC-94CB-6DCD48924DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{000A7D4E-9F12-4BA3-A5BC-7970D1E2066A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pcos_Recipes" sheetId="1" r:id="rId1"/>
@@ -9446,9 +9446,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="22.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -11034,7 +11036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="H170" sqref="H170"/>
     </sheetView>
   </sheetViews>

</xml_diff>